<commit_message>
Jan 19 - updates
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/advanced-deluxe20off-panelb.xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/advanced-deluxe20off-panelb.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23706"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{1E7725F7-393B-4DC3-AA51-013F1B91D1AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2AEF5BD-853C-4CCB-B700-D6E1395D1DB7}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{1E7725F7-393B-4DC3-AA51-013F1B91D1AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8BFA39FC-0931-4C7C-97D6-B56FA836288D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,7 +315,7 @@
     <t>Post Purchase Upsell Payment Plan (Installment)</t>
   </si>
   <si>
-    <t>ICSA346</t>
+    <t>ICSA36U</t>
   </si>
   <si>
     <t>ICSA347</t>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2571,21 +2571,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C47EEB8100460B478BDC3BCCBE3D5051" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829e995fc61fbfa25718206016b29da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2" xmlns:ns3="3e63a3be-2d53-41f2-914e-dd0efc332534" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3545440ad2b936a9d10385f8b267d779" ns2:_="" ns3:_="">
     <xsd:import namespace="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2"/>
@@ -2750,8 +2735,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFE8D63D-2E81-4339-837F-7F18C9494163}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59656202-A0B0-43EC-AE8C-F4D1B807D10E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2759,5 +2759,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59656202-A0B0-43EC-AE8C-F4D1B807D10E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFE8D63D-2E81-4339-837F-7F18C9494163}"/>
 </file>
</xml_diff>